<commit_message>
working on stock update release
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/StockTable.xlsx
+++ b/application/views/rpt/ru/StockTable.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iSell\www\isell\application\views\rpt\ru\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>п/п</t>
   </si>
@@ -75,24 +70,9 @@
     <t>{$v-&gt;stock-&gt;rows[]-&gt;product_volume}</t>
   </si>
   <si>
-    <t>{$v-&gt;stock-&gt;rows[]-&gt;party_label}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;stock-&gt;rows[]-&gt;product_uktzet}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;stock-&gt;rows[]-&gt;barcode}</t>
-  </si>
-  <si>
     <t>{$v-&gt;stock-&gt;rows[]-&gt;analyse_class}</t>
   </si>
   <si>
-    <t>{$v-&gt;stock-&gt;rows[]-&gt;analyse_group}</t>
-  </si>
-  <si>
-    <t>{$v-&gt;stock-&gt;rows[]-&gt;analyse_section}</t>
-  </si>
-  <si>
     <t>Ед</t>
   </si>
   <si>
@@ -126,24 +106,15 @@
     <t>Объем</t>
   </si>
   <si>
-    <t>Партия</t>
-  </si>
-  <si>
     <t>Штрихкод</t>
   </si>
   <si>
     <t>Тип</t>
   </si>
   <si>
-    <t>Группа</t>
-  </si>
-  <si>
     <t>Класс</t>
   </si>
   <si>
-    <t>Отдел</t>
-  </si>
-  <si>
     <t>Таблица склада ({$v-&gt;cat_name}) на {$v-&gt;date}</t>
   </si>
   <si>
@@ -160,6 +131,24 @@
   </si>
   <si>
     <t>{$v-&gt;stock-&gt;rows[]-&gt;analyse_type}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;stock-&gt;rows[]-&gt;analyse_origin}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;stock-&gt;rows[]-&gt;product_barcode}</t>
+  </si>
+  <si>
+    <t>Бренд</t>
+  </si>
+  <si>
+    <t>{$v-&gt;stock-&gt;rows[]-&gt;analyse_brand}</t>
+  </si>
+  <si>
+    <t>Артикул</t>
+  </si>
+  <si>
+    <t>{$v-&gt;stock-&gt;rows[]-&gt;product_article}</t>
   </si>
 </sst>
 </file>
@@ -219,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -348,11 +337,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -371,12 +386,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -402,13 +411,9 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="12" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,6 +423,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -489,7 +507,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -524,7 +542,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -733,54 +751,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="19.25" style="18" customWidth="1"/>
-    <col min="3" max="3" width="64.125" style="18" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="19" customWidth="1"/>
-    <col min="5" max="5" width="5.375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="10.75" style="18" customWidth="1"/>
-    <col min="7" max="17" width="9.125" style="18"/>
-    <col min="18" max="18" width="14.375" style="18" customWidth="1"/>
-    <col min="19" max="19" width="17.25" style="18" customWidth="1"/>
-    <col min="20" max="16384" width="9.125" style="18"/>
+    <col min="1" max="1" width="3.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="16" customWidth="1"/>
+    <col min="7" max="17" width="9.140625" style="16"/>
+    <col min="18" max="18" width="17.28515625" style="16" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
     </row>
-    <row r="2" spans="1:23" s="7" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="7" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -788,183 +804,176 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:23" s="28" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+    <row r="3" spans="1:22" s="24" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="23" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="S3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="5" t="s">
+      <c r="U3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="27" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="4" spans="1:23" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="20" t="s">
+      <c r="I4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="L4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="N4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="O4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="P4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="Q4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="R4" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="S4" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="V4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="W4" s="12" t="s">
-        <v>23</v>
+      <c r="T4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="17"/>
+    <row r="5" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="15"/>
     </row>
-    <row r="6" spans="1:23" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+    <row r="6" spans="1:22" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A1:V1"/>
     <mergeCell ref="B6:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D4">

</xml_diff>

<commit_message>
party_label in stock table
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/StockTable.xlsx
+++ b/application/views/rpt/ru/StockTable.xlsx
@@ -172,7 +172,7 @@
     <t xml:space="preserve">{$v-&gt;stock-&gt;rows[]-&gt;analyse_origin}</t>
   </si>
   <si>
-    <t xml:space="preserve">{$v→stock→rows[]→party_label}</t>
+    <t xml:space="preserve">{$v-&gt;stock-&gt;rows[]-&gt;party_label}</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,10 +453,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -579,20 +575,20 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA18" activeCellId="0" sqref="AA18"/>
+      <selection pane="topLeft" activeCell="AB16" activeCellId="0" sqref="AB16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="64.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="10.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="9" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="9" style="1" width="9.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="21" style="1" width="9.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="21" style="1" width="9.12"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +768,7 @@
       <c r="S4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="T4" s="19" t="s">
         <v>45</v>
       </c>
       <c r="U4" s="19" t="s">
@@ -784,50 +780,50 @@
       <c r="W4" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="X4" s="24" t="s">
+      <c r="X4" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="Y4" s="24" t="s">
+      <c r="Y4" s="23" t="s">
         <v>50</v>
       </c>
       <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="7" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28"/>
-      <c r="W5" s="28"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="29"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="28"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
       <c r="AMJ6" s="0"/>
     </row>
   </sheetData>

</xml_diff>